<commit_message>
Significantly streamlined cargo attachment functions and added echo handling system to combine designs
Crossbar functionality still not implemented in optical computers script
</commit_message>
<xml_diff>
--- a/core_plates/P2854_CW_seed_plug_center.xlsx
+++ b/core_plates/P2854_CW_seed_plug_center.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Documents/Shih_Lab_Postdoc/research_projects/crisscross_code/core_plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01060C9-4DE0-1E46-B684-219DE0A68296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB208A-2DBC-C84F-9608-D0561EB49FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -2804,7 +2804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="N7" sqref="J7:N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3598,11 +3600,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="9" width="43.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>